<commit_message>
Saturday 04 June 2022 04:36:32 PM IST
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -1,32 +1,63 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BANKING_SYSTEM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78351E14-F7FA-4015-A0E3-D415AF79B6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Account no.</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Father name</t>
+  </si>
+  <si>
+    <t>Security Pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balance </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,87 +76,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -413,111 +385,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6640625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="21.77734375" customWidth="1" style="1" min="1" max="1"/>
-    <col width="14.21875" customWidth="1" style="1" min="2" max="2"/>
-    <col width="16.88671875" customWidth="1" style="1" min="4" max="4"/>
-    <col width="17.33203125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="15.77734375" customWidth="1" style="1" min="6" max="6"/>
-    <col width="24.6640625" customWidth="1" style="1" min="7" max="7"/>
-    <col width="16.21875" customWidth="1" style="1" min="8" max="8"/>
+    <col min="1" max="1" width="21.77734375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.75" customHeight="1" s="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Account no.</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>DOB</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Gender</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Father name</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Security Pin</t>
-        </is>
-      </c>
-      <c r="G1" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Balance </t>
-        </is>
-      </c>
-      <c r="H1" s="3" t="n"/>
+    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3"/>
     </row>
-    <row r="2" ht="12.6" customHeight="1" s="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Shaik Roshan Ali</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>855111566</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>26/07/2004</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>M</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Shaik Rafic Ahammad</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>7602</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>3000</v>
-      </c>
+    <row r="2" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Friday 08 July 2022 11:30:49 PM IST
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BANKING_SYSTEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78351E14-F7FA-4015-A0E3-D415AF79B6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749CD4C9-D28D-4015-86A3-3AD15C39F732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -403,7 +403,7 @@
     <col min="8" max="8" width="16.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,13 +427,29 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="12.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="D2"/>
       <c r="E2"/>
       <c r="F2"/>
       <c r="G2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>

</xml_diff>

<commit_message>
Friday 08 July 2022 11:43:51 PM IST
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BANKING_SYSTEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749CD4C9-D28D-4015-86A3-3AD15C39F732}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3990B4A6-D926-4510-8397-FECFD2B9A29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -427,7 +427,7 @@
       </c>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2"/>
       <c r="B2"/>
       <c r="D2"/>
@@ -443,14 +443,6 @@
       <c r="F3"/>
       <c r="G3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Saturday 17 December 2022 07:06:37 PM IST
</commit_message>
<xml_diff>
--- a/accounts.xlsx
+++ b/accounts.xlsx
@@ -1,63 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BANKING_SYSTEM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3990B4A6-D926-4510-8397-FECFD2B9A29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Account no.</t>
-  </si>
-  <si>
-    <t>DOB</t>
-  </si>
-  <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Father name</t>
-  </si>
-  <si>
-    <t>Security Pin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Balance </t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <name val="Arial"/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -76,28 +45,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -385,70 +413,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="11.6640625" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="21.77734375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="14.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.21875" style="1" customWidth="1"/>
+    <col width="21.77734375" customWidth="1" style="1" min="1" max="1"/>
+    <col width="14.21875" customWidth="1" style="1" min="2" max="2"/>
+    <col width="16.88671875" customWidth="1" style="1" min="4" max="4"/>
+    <col width="17.33203125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="15.77734375" customWidth="1" style="1" min="6" max="6"/>
+    <col width="24.6640625" customWidth="1" style="1" min="7" max="7"/>
+    <col width="16.21875" customWidth="1" style="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3"/>
+    <row r="1" ht="13.2" customHeight="1" s="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Account no.</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>DOB</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Gender</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Father name</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Security Pin</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Balance </t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="n"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Manukonda Bhargav Krishna</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>5390768673</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>26/11/2003</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>M</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Manukonda Srinivasa Rao</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>8866</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>1000000</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>